<commit_message>
Adding this week materials
</commit_message>
<xml_diff>
--- a/Semester_1/Statistics_for_Data_Analytics/2_25_Sept_01_Oct_2023/Exercise_1_Descriptive_Stats.xlsx
+++ b/Semester_1/Statistics_for_Data_Analytics/2_25_Sept_01_Oct_2023/Exercise_1_Descriptive_Stats.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miant\Desktop\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/MSc_Data_Analytics_CCT_Materials/Semester_1/Statistics_for_Data_Analytics/2_25_Sept_01_Oct_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2F4482F-ABCD-4DC0-A633-A822DB635F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{D2F4482F-ABCD-4DC0-A633-A822DB635F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B18422E6-2107-431C-AA6C-CC271D52BF1B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6924BEAB-ADF4-47E8-A9B9-8E3CB548E4A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6924BEAB-ADF4-47E8-A9B9-8E3CB548E4A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$196</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1935,10 +1938,13 @@
   <dimension ref="A1:M196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C205" sqref="C205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -9935,6 +9941,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M196" xr:uid="{35E910E8-E9ED-4CDB-9337-EB3D50BE37F6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>